<commit_message>
fix importing claims whith unknown ,account number
</commit_message>
<xml_diff>
--- a/storage/app/public/excels/add-profils.xlsx
+++ b/storage/app/public/excels/add-profils.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">Le nom du profil concerné</t>
+    <t xml:space="preserve">Le nom du profil (le nom du rôle ) auquel on veut attribuer les nouveau rôles</t>
   </si>
   <si>
     <t xml:space="preserve">La liste des nouveaux rôles à attribuer aux utilisateurs ayant le profil concerné . Exemple (admin-pro/pilot-pro)</t>
@@ -120,12 +120,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -148,7 +148,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -161,15 +161,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating the customer import file
</commit_message>
<xml_diff>
--- a/storage/app/public/excels/add-profils.xlsx
+++ b/storage/app/public/excels/add-profils.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Le nom du profil concerné</t>
   </si>
   <si>
-    <t xml:space="preserve">La liste des nouveaux rôles à attribuer aux utilisateurs ayant le profil concerné . Exemple (admin-pro/pilot-pro)</t>
+    <t xml:space="preserve">La liste des nouveaux rôles à attribuer aux utilisateurs ayant le profil concerné . Exemple (admin-pro/pilot)</t>
   </si>
   <si>
     <t xml:space="preserve">profil</t>
@@ -148,7 +148,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>